<commit_message>
Added Salvage Value and Battery Replacement
</commit_message>
<xml_diff>
--- a/Results/Multi_Year/Battery_Data.xlsx
+++ b/Results/Multi_Year/Battery_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Dropbox\MicroGrids\TESI\MGP_Thesis_Version\Results\Multi_Year\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy-MYCE\Results\Multi_Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D87F742-087A-4CF5-9B5A-16C2F76DF044}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306587C1-D13F-4A48-9FEF-F596CC16F09A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5317" yWindow="3146" windowWidth="15951" windowHeight="8230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Unitary Investment Cost [USD/Wh]</t>
   </si>
@@ -35,12 +35,30 @@
     <t>Nominal Capacity at upgrade 1</t>
   </si>
   <si>
+    <t>Nominal Capacity at upgrade 2</t>
+  </si>
+  <si>
+    <t>Nominal Capacity at upgrade 3</t>
+  </si>
+  <si>
     <t>Investment at upgrade 1</t>
   </si>
   <si>
+    <t>Investment at upgrade 2</t>
+  </si>
+  <si>
+    <t>Investment at upgrade 3</t>
+  </si>
+  <si>
     <t>Yearly O&amp;M Cost at upgrade 1</t>
   </si>
   <si>
+    <t>Yearly O&amp;M Cost at upgrade 2</t>
+  </si>
+  <si>
+    <t>Yearly O&amp;M Cost at upgrade 3</t>
+  </si>
+  <si>
     <t>Total actualized Battery Reposition Cost</t>
   </si>
   <si>
@@ -54,57 +72,6 @@
   </si>
   <si>
     <t>Battery Reposition Cost at y = 3</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 4</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 5</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 6</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 7</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 8</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 9</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 10</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 11</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 12</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 13</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 14</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 15</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 16</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 17</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 18</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 19</t>
-  </si>
-  <si>
-    <t>Battery Reposition Cost at y = 20</t>
   </si>
 </sst>
 </file>
@@ -170,7 +137,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -186,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -506,14 +473,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -550,7 +517,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>528651.1469424807</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -558,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>236539.6691879436</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -566,7 +533,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4730.7933837588716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -574,7 +541,55 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>284541.33810564032</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -584,179 +599,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>13727.356752550369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>13895.25292252886</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>13938.534985693719</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>13982.080756168951</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>14019.00156241365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>14052.940248491959</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>14085.50899780086</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>14117.278038724049</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>14150.675355457681</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>14181.987593775901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>14221.14926785285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>14267.8982758975</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>14313.699816979501</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>14359.76804921334</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>14406.378397860581</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <v>14457.601615451311</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
-        <v>14506.11543113717</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <v>14567.72393755285</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20">
-        <v>14618.150169049361</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21">
-        <v>14672.235931042171</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MYCE_SalvageValue: removed Battery Replacement
</commit_message>
<xml_diff>
--- a/Results/Multi_Year/Battery_Data.xlsx
+++ b/Results/Multi_Year/Battery_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy-MYCE\Results\Multi_Year\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giulia\Desktop\MicroGridsPy_MYCE_SalvageValue\Results\Multi_Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306587C1-D13F-4A48-9FEF-F596CC16F09A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61FAA7DE-72C4-41FA-A900-A82062D088C9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Unitary Investment Cost [USD/Wh]</t>
   </si>
@@ -35,30 +35,12 @@
     <t>Nominal Capacity at upgrade 1</t>
   </si>
   <si>
-    <t>Nominal Capacity at upgrade 2</t>
-  </si>
-  <si>
-    <t>Nominal Capacity at upgrade 3</t>
-  </si>
-  <si>
     <t>Investment at upgrade 1</t>
   </si>
   <si>
-    <t>Investment at upgrade 2</t>
-  </si>
-  <si>
-    <t>Investment at upgrade 3</t>
-  </si>
-  <si>
     <t>Yearly O&amp;M Cost at upgrade 1</t>
   </si>
   <si>
-    <t>Yearly O&amp;M Cost at upgrade 2</t>
-  </si>
-  <si>
-    <t>Yearly O&amp;M Cost at upgrade 3</t>
-  </si>
-  <si>
     <t>Total actualized Battery Reposition Cost</t>
   </si>
   <si>
@@ -72,6 +54,12 @@
   </si>
   <si>
     <t>Battery Reposition Cost at y = 3</t>
+  </si>
+  <si>
+    <t>Battery Reposition Cost at y = 4</t>
+  </si>
+  <si>
+    <t>Battery Reposition Cost at y = 5</t>
   </si>
 </sst>
 </file>
@@ -473,30 +461,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.44744</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -504,92 +492,44 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.9715555555555553E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9.0348888888888883E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17418.989103017171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12890.05193623271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>257.80103872465418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
+        <v>4971.2525585970343</v>
       </c>
     </row>
   </sheetData>
@@ -599,43 +539,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>927.84386350063073</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>983.74473641765576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1019.887986226312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1019.887986226312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1019.887986226312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MYCE version employed for SDEWES
</commit_message>
<xml_diff>
--- a/Results/Multi_Year/Battery_Data.xlsx
+++ b/Results/Multi_Year/Battery_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy-MYCE\Results\Multi_Year\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Desktop\MicroGridsPy_MultiYearCapacityExpansion-Multi_Year_Capacity_Expansion\MicroGridsPy_MultiYearCapacityExpansion-Multi_Year_Capacity_Expansion\Results\Multi_Year\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306587C1-D13F-4A48-9FEF-F596CC16F09A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E40F7D-4B37-4EA1-96F0-7388F7026955}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5317" yWindow="3146" windowWidth="15951" windowHeight="8230" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery_Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Unitary Investment Cost [USD/Wh]</t>
   </si>
@@ -35,30 +35,12 @@
     <t>Nominal Capacity at upgrade 1</t>
   </si>
   <si>
-    <t>Nominal Capacity at upgrade 2</t>
-  </si>
-  <si>
-    <t>Nominal Capacity at upgrade 3</t>
-  </si>
-  <si>
     <t>Investment at upgrade 1</t>
   </si>
   <si>
-    <t>Investment at upgrade 2</t>
-  </si>
-  <si>
-    <t>Investment at upgrade 3</t>
-  </si>
-  <si>
     <t>Yearly O&amp;M Cost at upgrade 1</t>
   </si>
   <si>
-    <t>Yearly O&amp;M Cost at upgrade 2</t>
-  </si>
-  <si>
-    <t>Yearly O&amp;M Cost at upgrade 3</t>
-  </si>
-  <si>
     <t>Total actualized Battery Reposition Cost</t>
   </si>
   <si>
@@ -72,6 +54,12 @@
   </si>
   <si>
     <t>Battery Reposition Cost at y = 3</t>
+  </si>
+  <si>
+    <t>Battery Reposition Cost at y = 4</t>
+  </si>
+  <si>
+    <t>Battery Reposition Cost at y = 5</t>
   </si>
 </sst>
 </file>
@@ -137,7 +125,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -153,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -473,14 +461,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -517,7 +505,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>6175.0338886374811</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -525,7 +513,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>2762.957163131955</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -533,7 +521,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>55.259143262639093</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -541,55 +529,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
+        <v>144.6057673583835</v>
       </c>
     </row>
   </sheetData>
@@ -599,43 +539,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>72.376755136928352</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>42.342319963364957</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>21.39342939190227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2.3731693227008011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>6.1200935434860089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>